<commit_message>
MTP new xl for prod rel + icdc cart manifest
</commit_message>
<xml_diff>
--- a/InputFiles/MTP_DV3_22.11_v12.0.xlsx
+++ b/InputFiles/MTP_DV3_22.11_v12.0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/MTP (PPDC)/2-Executing/Input Test Data for DV3 Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B94AA182-3507-4C74-A30B-634953841672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_C28F3D7107EA371DEF8F0E8A8C37B8EC492352B8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE178315-F3C9-4054-9589-42C81965B601}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18870" yWindow="2805" windowWidth="24480" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sourceData" sheetId="1" r:id="rId1"/>
@@ -2472,23 +2472,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.7265625" customWidth="1"/>
-    <col min="2" max="2" width="20.7265625" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>45071.679765691937</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2563,9 +2563,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -2582,7 +2582,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -2616,7 +2616,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -2650,7 +2650,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -2667,7 +2667,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -2718,7 +2718,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -2786,7 +2786,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -2803,7 +2803,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -2820,7 +2820,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>2428</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>1804</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -2922,7 +2922,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -2956,7 +2956,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -2990,7 +2990,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>45</v>
       </c>
@@ -3075,7 +3075,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -3092,7 +3092,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -3126,7 +3126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>49</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>50</v>
       </c>
@@ -3160,7 +3160,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>51</v>
       </c>
@@ -3177,7 +3177,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>53</v>
       </c>
@@ -3211,7 +3211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>54</v>
       </c>
@@ -3228,7 +3228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>55</v>
       </c>
@@ -3245,7 +3245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>56</v>
       </c>
@@ -3272,12 +3272,15 @@
   <dimension ref="A1:N42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -3321,7 +3324,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>146</v>
       </c>
@@ -3365,7 +3368,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>147</v>
       </c>
@@ -3409,7 +3412,7 @@
         <v>6455</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>148</v>
       </c>
@@ -3453,7 +3456,7 @@
         <v>19274</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>149</v>
       </c>
@@ -3497,7 +3500,7 @@
         <v>3920</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>150</v>
       </c>
@@ -3541,7 +3544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>151</v>
       </c>
@@ -3585,7 +3588,7 @@
         <v>23212</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>152</v>
       </c>
@@ -3629,7 +3632,7 @@
         <v>6738</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>153</v>
       </c>
@@ -3673,7 +3676,7 @@
         <v>3002</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>154</v>
       </c>
@@ -3717,7 +3720,7 @@
         <v>48018</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>155</v>
       </c>
@@ -3761,7 +3764,7 @@
         <v>40415</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>156</v>
       </c>
@@ -3805,7 +3808,7 @@
         <v>19855</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>157</v>
       </c>
@@ -3849,7 +3852,7 @@
         <v>21268</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>158</v>
       </c>
@@ -3893,7 +3896,7 @@
         <v>14343</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>159</v>
       </c>
@@ -3937,7 +3940,7 @@
         <v>29224</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>160</v>
       </c>
@@ -3981,7 +3984,7 @@
         <v>3414</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>161</v>
       </c>
@@ -4025,7 +4028,7 @@
         <v>13629</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>162</v>
       </c>
@@ -4069,7 +4072,7 @@
         <v>13569</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>163</v>
       </c>
@@ -4113,7 +4116,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>164</v>
       </c>
@@ -4157,7 +4160,7 @@
         <v>8464</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>165</v>
       </c>
@@ -4201,7 +4204,7 @@
         <v>10209</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>166</v>
       </c>
@@ -4245,7 +4248,7 @@
         <v>2517</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>167</v>
       </c>
@@ -4289,7 +4292,7 @@
         <v>2152</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>168</v>
       </c>
@@ -4333,7 +4336,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>169</v>
       </c>
@@ -4377,7 +4380,7 @@
         <v>1437</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>170</v>
       </c>
@@ -4421,7 +4424,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>171</v>
       </c>
@@ -4465,7 +4468,7 @@
         <v>1663</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>172</v>
       </c>
@@ -4509,7 +4512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>173</v>
       </c>
@@ -4553,7 +4556,7 @@
         <v>13936</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>174</v>
       </c>
@@ -4597,7 +4600,7 @@
         <v>4794</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>175</v>
       </c>
@@ -4641,7 +4644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>176</v>
       </c>
@@ -4685,7 +4688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>177</v>
       </c>
@@ -4729,7 +4732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>178</v>
       </c>
@@ -4773,7 +4776,7 @@
         <v>15021</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>179</v>
       </c>
@@ -4817,7 +4820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>180</v>
       </c>
@@ -4861,7 +4864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>181</v>
       </c>
@@ -4905,7 +4908,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>182</v>
       </c>
@@ -4949,7 +4952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>183</v>
       </c>
@@ -4993,7 +4996,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>184</v>
       </c>
@@ -5037,7 +5040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>185</v>
       </c>
@@ -5081,7 +5084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>186</v>
       </c>
@@ -5134,11 +5137,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -5152,7 +5157,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>247</v>
       </c>
@@ -5166,7 +5171,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>248</v>
       </c>
@@ -5180,7 +5185,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>249</v>
       </c>
@@ -5194,7 +5199,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>250</v>
       </c>
@@ -5208,7 +5213,7 @@
         <v>7751</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>251</v>
       </c>
@@ -5222,7 +5227,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>252</v>
       </c>
@@ -5236,7 +5241,7 @@
         <v>2169</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>253</v>
       </c>
@@ -5250,7 +5255,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>254</v>
       </c>
@@ -5264,7 +5269,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>255</v>
       </c>
@@ -5278,7 +5283,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>256</v>
       </c>
@@ -5292,7 +5297,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>257</v>
       </c>
@@ -5306,7 +5311,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>258</v>
       </c>
@@ -5320,7 +5325,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>259</v>
       </c>
@@ -5334,7 +5339,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>260</v>
       </c>
@@ -5348,7 +5353,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>261</v>
       </c>
@@ -5362,7 +5367,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>262</v>
       </c>
@@ -5376,7 +5381,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>263</v>
       </c>
@@ -5390,7 +5395,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>264</v>
       </c>
@@ -5404,7 +5409,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>265</v>
       </c>
@@ -5418,7 +5423,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>266</v>
       </c>
@@ -5432,7 +5437,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>267</v>
       </c>
@@ -5446,7 +5451,7 @@
         <v>2631</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>268</v>
       </c>
@@ -5460,7 +5465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>269</v>
       </c>
@@ -5474,7 +5479,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>270</v>
       </c>
@@ -5488,7 +5493,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>271</v>
       </c>
@@ -5502,7 +5507,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>272</v>
       </c>
@@ -5516,7 +5521,7 @@
         <v>1451</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>273</v>
       </c>
@@ -5530,7 +5535,7 @@
         <v>4299</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>274</v>
       </c>
@@ -5544,7 +5549,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>275</v>
       </c>
@@ -5558,7 +5563,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>276</v>
       </c>
@@ -5572,7 +5577,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>277</v>
       </c>
@@ -5586,7 +5591,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>278</v>
       </c>
@@ -5600,7 +5605,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>279</v>
       </c>
@@ -5614,7 +5619,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>280</v>
       </c>
@@ -5628,7 +5633,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>281</v>
       </c>
@@ -5642,7 +5647,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>282</v>
       </c>
@@ -5656,7 +5661,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>283</v>
       </c>
@@ -5670,7 +5675,7 @@
         <v>1823</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>284</v>
       </c>
@@ -5684,7 +5689,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>285</v>
       </c>
@@ -5698,7 +5703,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>286</v>
       </c>
@@ -5712,7 +5717,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>287</v>
       </c>
@@ -5726,7 +5731,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>288</v>
       </c>
@@ -5740,7 +5745,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>289</v>
       </c>
@@ -5754,7 +5759,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>290</v>
       </c>
@@ -5768,7 +5773,7 @@
         <v>5068</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>291</v>
       </c>
@@ -5782,7 +5787,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>292</v>
       </c>
@@ -5796,7 +5801,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>293</v>
       </c>
@@ -5810,7 +5815,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>294</v>
       </c>
@@ -5824,7 +5829,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>295</v>
       </c>
@@ -5838,7 +5843,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>296</v>
       </c>
@@ -5852,7 +5857,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>297</v>
       </c>
@@ -5866,7 +5871,7 @@
         <v>4249</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>298</v>
       </c>
@@ -5880,7 +5885,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>299</v>
       </c>
@@ -5894,7 +5899,7 @@
         <v>3752</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>300</v>
       </c>
@@ -5908,7 +5913,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>301</v>
       </c>
@@ -5922,7 +5927,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>302</v>
       </c>
@@ -5936,7 +5941,7 @@
         <v>5544</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>303</v>
       </c>
@@ -5950,7 +5955,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>304</v>
       </c>
@@ -5964,7 +5969,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>305</v>
       </c>
@@ -5978,7 +5983,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>306</v>
       </c>
@@ -5992,7 +5997,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>307</v>
       </c>
@@ -6006,7 +6011,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>308</v>
       </c>
@@ -6020,7 +6025,7 @@
         <v>6848</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>309</v>
       </c>
@@ -6034,7 +6039,7 @@
         <v>2866</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>310</v>
       </c>
@@ -6048,7 +6053,7 @@
         <v>5684</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>311</v>
       </c>
@@ -6062,7 +6067,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>312</v>
       </c>
@@ -6076,7 +6081,7 @@
         <v>1444</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>313</v>
       </c>
@@ -6090,7 +6095,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>314</v>
       </c>
@@ -6104,7 +6109,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>315</v>
       </c>
@@ -6118,7 +6123,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>316</v>
       </c>
@@ -6132,7 +6137,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>317</v>
       </c>
@@ -6146,7 +6151,7 @@
         <v>7109</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>318</v>
       </c>
@@ -6160,7 +6165,7 @@
         <v>7008</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>319</v>
       </c>
@@ -6174,7 +6179,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>320</v>
       </c>
@@ -6188,7 +6193,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>321</v>
       </c>
@@ -6202,7 +6207,7 @@
         <v>7207</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>322</v>
       </c>
@@ -6216,7 +6221,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>323</v>
       </c>
@@ -6230,7 +6235,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>324</v>
       </c>
@@ -6244,7 +6249,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>325</v>
       </c>
@@ -6269,9 +6274,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -6285,7 +6290,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>485</v>
       </c>
@@ -6299,7 +6304,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>486</v>
       </c>
@@ -6313,7 +6318,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>487</v>
       </c>
@@ -6327,7 +6332,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>488</v>
       </c>
@@ -6341,7 +6346,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>489</v>
       </c>
@@ -6355,7 +6360,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>490</v>
       </c>
@@ -6369,7 +6374,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>491</v>
       </c>
@@ -6383,7 +6388,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>492</v>
       </c>
@@ -6397,7 +6402,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>493</v>
       </c>
@@ -6411,7 +6416,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>494</v>
       </c>
@@ -6425,7 +6430,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>495</v>
       </c>
@@ -6439,7 +6444,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>496</v>
       </c>
@@ -6453,7 +6458,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>497</v>
       </c>
@@ -6467,7 +6472,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>498</v>
       </c>
@@ -6481,7 +6486,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>499</v>
       </c>
@@ -6495,7 +6500,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>500</v>
       </c>
@@ -6509,7 +6514,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>501</v>
       </c>
@@ -6523,7 +6528,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>502</v>
       </c>
@@ -6537,7 +6542,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>503</v>
       </c>
@@ -6551,7 +6556,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>504</v>
       </c>
@@ -6565,7 +6570,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>505</v>
       </c>
@@ -6579,7 +6584,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>506</v>
       </c>
@@ -6593,7 +6598,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>507</v>
       </c>
@@ -6607,7 +6612,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>508</v>
       </c>
@@ -6621,7 +6626,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>509</v>
       </c>
@@ -6635,7 +6640,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>510</v>
       </c>
@@ -6649,7 +6654,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>511</v>
       </c>
@@ -6663,7 +6668,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>512</v>
       </c>
@@ -6677,7 +6682,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>513</v>
       </c>
@@ -6691,7 +6696,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>514</v>
       </c>
@@ -6705,7 +6710,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>515</v>
       </c>
@@ -6719,7 +6724,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>516</v>
       </c>
@@ -6733,7 +6738,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>517</v>
       </c>
@@ -6747,7 +6752,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>518</v>
       </c>
@@ -6761,7 +6766,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>519</v>
       </c>
@@ -6775,7 +6780,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>520</v>
       </c>
@@ -6789,7 +6794,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>521</v>
       </c>
@@ -6803,7 +6808,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>522</v>
       </c>
@@ -6817,7 +6822,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>523</v>
       </c>
@@ -6831,7 +6836,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>524</v>
       </c>
@@ -6845,7 +6850,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>525</v>
       </c>
@@ -6859,7 +6864,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>526</v>
       </c>
@@ -6873,7 +6878,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>527</v>
       </c>
@@ -6887,7 +6892,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>528</v>
       </c>
@@ -6901,7 +6906,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>529</v>
       </c>
@@ -6915,7 +6920,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>530</v>
       </c>
@@ -6929,7 +6934,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>531</v>
       </c>
@@ -6943,7 +6948,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>532</v>
       </c>
@@ -6957,7 +6962,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>533</v>
       </c>
@@ -6971,7 +6976,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>534</v>
       </c>
@@ -6985,7 +6990,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>535</v>
       </c>
@@ -6999,7 +7004,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>536</v>
       </c>
@@ -7013,7 +7018,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>537</v>
       </c>
@@ -7027,7 +7032,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>538</v>
       </c>
@@ -7041,7 +7046,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>539</v>
       </c>
@@ -7055,7 +7060,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>540</v>
       </c>
@@ -7069,7 +7074,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>541</v>
       </c>
@@ -7083,7 +7088,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>542</v>
       </c>
@@ -7097,7 +7102,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>543</v>
       </c>
@@ -7111,7 +7116,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>544</v>
       </c>
@@ -7125,7 +7130,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>545</v>
       </c>
@@ -7139,7 +7144,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>546</v>
       </c>
@@ -7153,7 +7158,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>547</v>
       </c>
@@ -7167,7 +7172,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>548</v>
       </c>
@@ -7191,15 +7196,15 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="37.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -7246,7 +7251,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>550</v>
       </c>
@@ -7293,7 +7298,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>551</v>
       </c>
@@ -7340,7 +7345,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>552</v>
       </c>
@@ -7387,7 +7392,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>553</v>
       </c>
@@ -7434,7 +7439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>554</v>
       </c>
@@ -7481,7 +7486,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>555</v>
       </c>
@@ -7528,7 +7533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>556</v>
       </c>
@@ -7575,7 +7580,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>557</v>
       </c>
@@ -7622,7 +7627,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>558</v>
       </c>
@@ -7669,7 +7674,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>559</v>
       </c>
@@ -7716,7 +7721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>560</v>
       </c>
@@ -7763,7 +7768,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>561</v>
       </c>
@@ -7810,7 +7815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>562</v>
       </c>
@@ -7857,7 +7862,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>563</v>
       </c>
@@ -7904,7 +7909,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>564</v>
       </c>
@@ -7951,7 +7956,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>565</v>
       </c>
@@ -7998,7 +8003,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>566</v>
       </c>
@@ -8045,7 +8050,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>567</v>
       </c>
@@ -8092,7 +8097,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>568</v>
       </c>
@@ -8139,7 +8144,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>569</v>
       </c>
@@ -8186,7 +8191,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>570</v>
       </c>
@@ -8233,7 +8238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>571</v>
       </c>
@@ -8280,7 +8285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>572</v>
       </c>
@@ -8327,7 +8332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>573</v>
       </c>
@@ -8374,7 +8379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>574</v>
       </c>
@@ -8421,7 +8426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>575</v>
       </c>
@@ -8468,7 +8473,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>576</v>
       </c>
@@ -8515,7 +8520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>577</v>
       </c>
@@ -8562,7 +8567,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>578</v>
       </c>
@@ -8609,7 +8614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>579</v>
       </c>
@@ -8656,7 +8661,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>580</v>
       </c>
@@ -8703,7 +8708,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>581</v>
       </c>
@@ -8750,7 +8755,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>582</v>
       </c>
@@ -8797,7 +8802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>583</v>
       </c>
@@ -8844,7 +8849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>584</v>
       </c>
@@ -8891,7 +8896,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>585</v>
       </c>
@@ -8938,7 +8943,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>586</v>
       </c>
@@ -8985,7 +8990,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>587</v>
       </c>
@@ -9032,7 +9037,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>588</v>
       </c>
@@ -9079,7 +9084,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>589</v>
       </c>
@@ -9135,11 +9140,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -9153,7 +9158,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>652</v>
       </c>
@@ -9167,7 +9172,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>652</v>
       </c>
@@ -9181,7 +9186,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>652</v>
       </c>
@@ -9195,7 +9200,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>652</v>
       </c>
@@ -9209,7 +9214,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>652</v>
       </c>
@@ -9223,7 +9228,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>652</v>
       </c>
@@ -9237,7 +9242,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>652</v>
       </c>
@@ -9251,7 +9256,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>652</v>
       </c>
@@ -9265,7 +9270,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>652</v>
       </c>
@@ -9279,7 +9284,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>652</v>
       </c>
@@ -9293,7 +9298,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>652</v>
       </c>
@@ -9307,7 +9312,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>652</v>
       </c>
@@ -9321,7 +9326,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>652</v>
       </c>
@@ -9335,7 +9340,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>652</v>
       </c>
@@ -9349,7 +9354,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>652</v>
       </c>
@@ -9363,7 +9368,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>652</v>
       </c>
@@ -9377,7 +9382,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>652</v>
       </c>
@@ -9391,7 +9396,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>652</v>
       </c>
@@ -9405,7 +9410,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>652</v>
       </c>
@@ -9419,7 +9424,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>652</v>
       </c>
@@ -9433,7 +9438,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>652</v>
       </c>
@@ -9447,7 +9452,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>652</v>
       </c>
@@ -9461,7 +9466,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>652</v>
       </c>
@@ -9475,7 +9480,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>652</v>
       </c>
@@ -9489,7 +9494,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>652</v>
       </c>
@@ -9503,7 +9508,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>652</v>
       </c>
@@ -9517,7 +9522,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>652</v>
       </c>
@@ -9531,7 +9536,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>652</v>
       </c>
@@ -9545,7 +9550,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>652</v>
       </c>
@@ -9559,7 +9564,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>652</v>
       </c>
@@ -9573,7 +9578,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>652</v>
       </c>
@@ -9587,7 +9592,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>652</v>
       </c>
@@ -9601,7 +9606,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>652</v>
       </c>
@@ -9615,7 +9620,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>652</v>
       </c>
@@ -9629,7 +9634,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>652</v>
       </c>
@@ -9643,7 +9648,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>652</v>
       </c>
@@ -9657,7 +9662,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>652</v>
       </c>
@@ -9671,7 +9676,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>652</v>
       </c>
@@ -9685,7 +9690,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>652</v>
       </c>
@@ -9699,7 +9704,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>652</v>
       </c>
@@ -9713,7 +9718,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>652</v>
       </c>
@@ -9738,9 +9743,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -9754,7 +9759,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>652</v>
       </c>
@@ -9768,7 +9773,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>652</v>
       </c>
@@ -9782,7 +9787,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>652</v>
       </c>
@@ -9796,7 +9801,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>652</v>
       </c>
@@ -9810,7 +9815,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>652</v>
       </c>
@@ -9824,7 +9829,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>652</v>
       </c>
@@ -9838,7 +9843,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>652</v>
       </c>
@@ -9852,7 +9857,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>652</v>
       </c>
@@ -9866,7 +9871,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>652</v>
       </c>
@@ -9880,7 +9885,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>652</v>
       </c>
@@ -9894,7 +9899,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>652</v>
       </c>
@@ -9908,7 +9913,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>652</v>
       </c>
@@ -9922,7 +9927,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>652</v>
       </c>
@@ -9936,7 +9941,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>652</v>
       </c>
@@ -9950,7 +9955,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>652</v>
       </c>
@@ -9964,7 +9969,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>652</v>
       </c>
@@ -9978,7 +9983,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>652</v>
       </c>
@@ -9992,7 +9997,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>652</v>
       </c>
@@ -10006,7 +10011,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>652</v>
       </c>
@@ -10020,7 +10025,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>652</v>
       </c>
@@ -10034,7 +10039,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>652</v>
       </c>
@@ -10048,7 +10053,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>652</v>
       </c>
@@ -10062,7 +10067,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>652</v>
       </c>
@@ -10076,7 +10081,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>652</v>
       </c>
@@ -10090,7 +10095,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>652</v>
       </c>
@@ -10104,7 +10109,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>652</v>
       </c>
@@ -10118,7 +10123,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>652</v>
       </c>
@@ -10132,7 +10137,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>652</v>
       </c>
@@ -10146,7 +10151,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>652</v>
       </c>
@@ -10160,7 +10165,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>652</v>
       </c>
@@ -10174,7 +10179,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>652</v>
       </c>
@@ -10188,7 +10193,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>652</v>
       </c>
@@ -10202,7 +10207,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>652</v>
       </c>
@@ -10216,7 +10221,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>652</v>
       </c>
@@ -10230,7 +10235,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>652</v>
       </c>
@@ -10255,9 +10260,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -10271,7 +10276,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>676</v>
       </c>
@@ -10285,7 +10290,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>676</v>
       </c>
@@ -10305,6 +10310,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d255e04af8190f6c31f5773ad84c428e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a8a25e01f7003c922a76e9f426634f46" ns2:_="" ns3:_="">
     <xsd:import namespace="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
@@ -10533,27 +10558,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77B5D4CA-FB9E-4D01-8E29-8CFF7CD858D9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF9BB7A6-BE2E-4B6D-8EC7-2FAADC1EC7C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D09680B-4ACC-4615-A766-70DEF14FBB11}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10570,35 +10600,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF9BB7A6-BE2E-4B6D-8EC7-2FAADC1EC7C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77B5D4CA-FB9E-4D01-8E29-8CFF7CD858D9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
-<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{14b77578-9773-42d5-8507-251ca2dc2b06}" enabled="0" method="" siteId="{14b77578-9773-42d5-8507-251ca2dc2b06}" removed="1"/>
-</clbl:labelList>
 </file>
</xml_diff>